<commit_message>
start on tables and plots
</commit_message>
<xml_diff>
--- a/2023/SAFE/other/HistModelSSB.xlsx
+++ b/2023/SAFE/other/HistModelSSB.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA - PH Stuff\2022 Assmnts\PCod\goa_pcod\SAFE\Other materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AA - PH Stuff\Asmnts\goa_pcod\2023\safe\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="0" windowWidth="21240" windowHeight="11240"/>
+    <workbookView xWindow="3750" yWindow="0" windowWidth="21240" windowHeight="11235"/>
   </bookViews>
   <sheets>
     <sheet name="SPBIOM_chart" sheetId="13" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>2020 M19.1</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>2022 M19.1a</t>
+  </si>
+  <si>
+    <t>2023 M19.1b</t>
   </si>
 </sst>
 </file>
@@ -88,7 +91,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -102,6 +105,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6639,6 +6643,210 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B808-4FF4-B802-AFBBD5187A74}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="20"/>
+          <c:order val="20"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2023 M19.1b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="80000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$V$2:$V$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>86688.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98379.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97763.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96006.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>111789</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>134329.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145537.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>149802</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>168636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>197792.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>220913.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>231754.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>243438.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>246919</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>230939</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>214700</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>201963.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>207131.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>211697</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>194439</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>169657</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>142072</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>125720.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>108573</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>95796</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>88197.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>82954.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>84857</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>82850</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>76512</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>68076</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>63091.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>67152.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>86781.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>99472</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>107730.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>114120.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>118695</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>86061.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>70065.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>53898</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>47454</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>48468.15</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>51108</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>59590</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>61227.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>55169.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>51959</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-30D0-4832-B80D-F1E5EA85D97D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6809,10 +7017,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="1.6685979329831343E-2"/>
-          <c:y val="0.84842214743050992"/>
-          <c:w val="0.96815223304880826"/>
-          <c:h val="0.13948028249364566"/>
+          <c:x val="2.5482668806807572E-2"/>
+          <c:y val="0.84842213712964498"/>
+          <c:w val="0.96756448994604016"/>
+          <c:h val="0.15157786287035507"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -7415,7 +7623,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -7427,7 +7635,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660984" cy="6282336"/>
+    <xdr:ext cx="8662358" cy="6272123"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -7713,20 +7921,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM48"/>
+  <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:U48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="12.453125" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>2003</v>
       </c>
@@ -7787,8 +7995,11 @@
       <c r="U1" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="V1" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1977</v>
       </c>
@@ -7851,11 +8062,14 @@
       </c>
       <c r="U2">
         <v>92966.5</v>
+      </c>
+      <c r="V2">
+        <v>86688.5</v>
       </c>
       <c r="W2" s="2"/>
       <c r="AM2" s="1"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1978</v>
       </c>
@@ -7919,11 +8133,13 @@
       <c r="U3">
         <v>104326</v>
       </c>
-      <c r="V3" s="2"/>
+      <c r="V3">
+        <v>98379.5</v>
+      </c>
       <c r="W3" s="2"/>
       <c r="AM3" s="1"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1979</v>
       </c>
@@ -7987,11 +8203,13 @@
       <c r="U4">
         <v>102381</v>
       </c>
-      <c r="V4" s="2"/>
+      <c r="V4">
+        <v>97763.5</v>
+      </c>
       <c r="W4" s="2"/>
       <c r="AM4" s="1"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1980</v>
       </c>
@@ -8055,11 +8273,13 @@
       <c r="U5">
         <v>100289.5</v>
       </c>
-      <c r="V5" s="2"/>
+      <c r="V5">
+        <v>96006.5</v>
+      </c>
       <c r="W5" s="2"/>
       <c r="AM5" s="1"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1981</v>
       </c>
@@ -8123,11 +8343,13 @@
       <c r="U6">
         <v>119195.5</v>
       </c>
-      <c r="V6" s="2"/>
+      <c r="V6">
+        <v>111789</v>
+      </c>
       <c r="W6" s="2"/>
       <c r="AM6" s="1"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1982</v>
       </c>
@@ -8191,11 +8413,13 @@
       <c r="U7">
         <v>143623</v>
       </c>
-      <c r="V7" s="2"/>
+      <c r="V7">
+        <v>134329.5</v>
+      </c>
       <c r="W7" s="2"/>
       <c r="AM7" s="1"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1983</v>
       </c>
@@ -8259,11 +8483,13 @@
       <c r="U8">
         <v>153763</v>
       </c>
-      <c r="V8" s="2"/>
+      <c r="V8">
+        <v>145537.5</v>
+      </c>
       <c r="W8" s="2"/>
       <c r="AM8" s="1"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1984</v>
       </c>
@@ -8327,11 +8553,13 @@
       <c r="U9">
         <v>156225.5</v>
       </c>
-      <c r="V9" s="2"/>
+      <c r="V9">
+        <v>149802</v>
+      </c>
       <c r="W9" s="2"/>
       <c r="AM9" s="1"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1985</v>
       </c>
@@ -8395,11 +8623,13 @@
       <c r="U10">
         <v>174891</v>
       </c>
-      <c r="V10" s="2"/>
+      <c r="V10">
+        <v>168636</v>
+      </c>
       <c r="W10" s="2"/>
       <c r="AM10" s="1"/>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1986</v>
       </c>
@@ -8463,11 +8693,13 @@
       <c r="U11">
         <v>204307.5</v>
       </c>
-      <c r="V11" s="2"/>
+      <c r="V11">
+        <v>197792.5</v>
+      </c>
       <c r="W11" s="2"/>
       <c r="AM11" s="1"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1987</v>
       </c>
@@ -8531,11 +8763,13 @@
       <c r="U12">
         <v>227282</v>
       </c>
-      <c r="V12" s="2"/>
+      <c r="V12">
+        <v>220913.5</v>
+      </c>
       <c r="W12" s="2"/>
       <c r="AM12" s="1"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1988</v>
       </c>
@@ -8599,11 +8833,13 @@
       <c r="U13">
         <v>236673</v>
       </c>
-      <c r="V13" s="2"/>
+      <c r="V13">
+        <v>231754.5</v>
+      </c>
       <c r="W13" s="2"/>
       <c r="AM13" s="1"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1989</v>
       </c>
@@ -8667,11 +8903,13 @@
       <c r="U14">
         <v>246814</v>
       </c>
-      <c r="V14" s="2"/>
+      <c r="V14">
+        <v>243438.5</v>
+      </c>
       <c r="W14" s="2"/>
       <c r="AM14" s="1"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1990</v>
       </c>
@@ -8735,11 +8973,13 @@
       <c r="U15">
         <v>248159</v>
       </c>
-      <c r="V15" s="2"/>
+      <c r="V15">
+        <v>246919</v>
+      </c>
       <c r="W15" s="2"/>
       <c r="AM15" s="1"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1991</v>
       </c>
@@ -8803,11 +9043,13 @@
       <c r="U16">
         <v>230387.5</v>
       </c>
-      <c r="V16" s="2"/>
+      <c r="V16">
+        <v>230939</v>
+      </c>
       <c r="W16" s="2"/>
       <c r="AM16" s="1"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1992</v>
       </c>
@@ -8871,11 +9113,13 @@
       <c r="U17">
         <v>213000.5</v>
       </c>
-      <c r="V17" s="2"/>
+      <c r="V17">
+        <v>214700</v>
+      </c>
       <c r="W17" s="2"/>
       <c r="AM17" s="1"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1993</v>
       </c>
@@ -8939,11 +9183,13 @@
       <c r="U18">
         <v>200365</v>
       </c>
-      <c r="V18" s="2"/>
+      <c r="V18">
+        <v>201963.5</v>
+      </c>
       <c r="W18" s="2"/>
       <c r="AM18" s="1"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1994</v>
       </c>
@@ -9007,11 +9253,13 @@
       <c r="U19">
         <v>205996</v>
       </c>
-      <c r="V19" s="2"/>
+      <c r="V19">
+        <v>207131.5</v>
+      </c>
       <c r="W19" s="2"/>
       <c r="AM19" s="1"/>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1995</v>
       </c>
@@ -9075,11 +9323,13 @@
       <c r="U20">
         <v>210226.5</v>
       </c>
-      <c r="V20" s="2"/>
+      <c r="V20">
+        <v>211697</v>
+      </c>
       <c r="W20" s="2"/>
       <c r="AM20" s="1"/>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1996</v>
       </c>
@@ -9143,11 +9393,13 @@
       <c r="U21">
         <v>192334.5</v>
       </c>
-      <c r="V21" s="2"/>
+      <c r="V21">
+        <v>194439</v>
+      </c>
       <c r="W21" s="2"/>
       <c r="AM21" s="1"/>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1997</v>
       </c>
@@ -9211,11 +9463,13 @@
       <c r="U22">
         <v>166601.5</v>
       </c>
-      <c r="V22" s="2"/>
+      <c r="V22">
+        <v>169657</v>
+      </c>
       <c r="W22" s="2"/>
       <c r="AM22" s="1"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1998</v>
       </c>
@@ -9279,11 +9533,13 @@
       <c r="U23">
         <v>138252.5</v>
       </c>
-      <c r="V23" s="2"/>
+      <c r="V23">
+        <v>142072</v>
+      </c>
       <c r="W23" s="2"/>
       <c r="AM23" s="1"/>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1999</v>
       </c>
@@ -9347,11 +9603,13 @@
       <c r="U24">
         <v>122006.5</v>
       </c>
-      <c r="V24" s="2"/>
+      <c r="V24">
+        <v>125720.5</v>
+      </c>
       <c r="W24" s="2"/>
       <c r="AM24" s="1"/>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2000</v>
       </c>
@@ -9415,11 +9673,13 @@
       <c r="U25">
         <v>104987.5</v>
       </c>
-      <c r="V25" s="2"/>
+      <c r="V25">
+        <v>108573</v>
+      </c>
       <c r="W25" s="2"/>
       <c r="AM25" s="1"/>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2001</v>
       </c>
@@ -9483,11 +9743,13 @@
       <c r="U26">
         <v>92439</v>
       </c>
-      <c r="V26" s="2"/>
+      <c r="V26">
+        <v>95796</v>
+      </c>
       <c r="W26" s="2"/>
       <c r="AM26" s="1"/>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2002</v>
       </c>
@@ -9551,11 +9813,13 @@
       <c r="U27">
         <v>84865.5</v>
       </c>
-      <c r="V27" s="2"/>
+      <c r="V27">
+        <v>88197.5</v>
+      </c>
       <c r="W27" s="2"/>
       <c r="AM27" s="1"/>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2003</v>
       </c>
@@ -9616,11 +9880,13 @@
       <c r="U28">
         <v>79759</v>
       </c>
-      <c r="V28" s="2"/>
+      <c r="V28">
+        <v>82954.5</v>
+      </c>
       <c r="W28" s="2"/>
       <c r="AM28" s="1"/>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2004</v>
       </c>
@@ -9678,11 +9944,13 @@
       <c r="U29">
         <v>81894.5</v>
       </c>
-      <c r="V29" s="2"/>
+      <c r="V29">
+        <v>84857</v>
+      </c>
       <c r="W29" s="2"/>
       <c r="AM29" s="1"/>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2005</v>
       </c>
@@ -9740,11 +10008,13 @@
       <c r="U30">
         <v>79790</v>
       </c>
-      <c r="V30" s="2"/>
+      <c r="V30">
+        <v>82850</v>
+      </c>
       <c r="W30" s="2"/>
       <c r="AM30" s="1"/>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2006</v>
       </c>
@@ -9799,11 +10069,13 @@
       <c r="U31">
         <v>73028.5</v>
       </c>
-      <c r="V31" s="2"/>
+      <c r="V31">
+        <v>76512</v>
+      </c>
       <c r="W31" s="2"/>
       <c r="AM31" s="1"/>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2007</v>
       </c>
@@ -9855,11 +10127,13 @@
       <c r="U32">
         <v>64425</v>
       </c>
-      <c r="V32" s="2"/>
+      <c r="V32">
+        <v>68076</v>
+      </c>
       <c r="W32" s="2"/>
       <c r="AM32" s="1"/>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2008</v>
       </c>
@@ -9911,11 +10185,13 @@
       <c r="U33">
         <v>59571.5</v>
       </c>
-      <c r="V33" s="2"/>
+      <c r="V33">
+        <v>63091.5</v>
+      </c>
       <c r="W33" s="2"/>
       <c r="AM33" s="1"/>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2009</v>
       </c>
@@ -9964,11 +10240,13 @@
       <c r="U34">
         <v>64239</v>
       </c>
-      <c r="V34" s="2"/>
+      <c r="V34">
+        <v>67152.5</v>
+      </c>
       <c r="W34" s="2"/>
       <c r="AM34" s="1"/>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2010</v>
       </c>
@@ -10011,11 +10289,13 @@
       <c r="U35">
         <v>84633.5</v>
       </c>
-      <c r="V35" s="2"/>
+      <c r="V35">
+        <v>86781.5</v>
+      </c>
       <c r="W35" s="2"/>
       <c r="AM35" s="1"/>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2011</v>
       </c>
@@ -10058,11 +10338,13 @@
       <c r="U36">
         <v>96908.5</v>
       </c>
-      <c r="V36" s="2"/>
+      <c r="V36">
+        <v>99472</v>
+      </c>
       <c r="W36" s="2"/>
       <c r="AM36" s="1"/>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2012</v>
       </c>
@@ -10102,11 +10384,13 @@
       <c r="U37">
         <v>104694.5</v>
       </c>
-      <c r="V37" s="2"/>
+      <c r="V37">
+        <v>107730.5</v>
+      </c>
       <c r="W37" s="2"/>
       <c r="AM37" s="1"/>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2013</v>
       </c>
@@ -10143,11 +10427,13 @@
       <c r="U38">
         <v>110162</v>
       </c>
-      <c r="V38" s="2"/>
+      <c r="V38">
+        <v>114120.5</v>
+      </c>
       <c r="W38" s="2"/>
       <c r="AM38" s="1"/>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2014</v>
       </c>
@@ -10184,11 +10470,13 @@
       <c r="U39">
         <v>114924</v>
       </c>
-      <c r="V39" s="2"/>
+      <c r="V39">
+        <v>118695</v>
+      </c>
       <c r="W39" s="2"/>
       <c r="AM39" s="1"/>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2015</v>
       </c>
@@ -10218,11 +10506,14 @@
       </c>
       <c r="U40">
         <v>82364.5</v>
+      </c>
+      <c r="V40">
+        <v>86061.5</v>
       </c>
       <c r="W40" s="2"/>
       <c r="AM40" s="1"/>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2016</v>
       </c>
@@ -10249,11 +10540,14 @@
       </c>
       <c r="U41">
         <v>66547</v>
+      </c>
+      <c r="V41">
+        <v>70065.5</v>
       </c>
       <c r="W41" s="2"/>
       <c r="AM41" s="1"/>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2017</v>
       </c>
@@ -10278,9 +10572,12 @@
       <c r="U42">
         <v>49557.3</v>
       </c>
+      <c r="V42">
+        <v>53898</v>
+      </c>
       <c r="AM42" s="1"/>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2018</v>
       </c>
@@ -10302,9 +10599,12 @@
       <c r="U43">
         <v>42244.75</v>
       </c>
+      <c r="V43">
+        <v>47454</v>
+      </c>
       <c r="AM43" s="1"/>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2019</v>
       </c>
@@ -10324,9 +10624,12 @@
       <c r="U44">
         <v>42175.45</v>
       </c>
+      <c r="V44">
+        <v>48468.15</v>
+      </c>
       <c r="AM44" s="1"/>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2020</v>
       </c>
@@ -10343,9 +10646,12 @@
       <c r="U45">
         <v>43895.85</v>
       </c>
+      <c r="V45">
+        <v>51108</v>
+      </c>
       <c r="AM45" s="1"/>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2021</v>
       </c>
@@ -10359,9 +10665,12 @@
       <c r="U46">
         <v>51289</v>
       </c>
+      <c r="V46">
+        <v>59590</v>
+      </c>
       <c r="AM46" s="1"/>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2022</v>
       </c>
@@ -10372,9 +10681,12 @@
       <c r="U47">
         <v>51733.5</v>
       </c>
+      <c r="V47">
+        <v>61227.5</v>
+      </c>
       <c r="AM47" s="1"/>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2023</v>
       </c>
@@ -10382,7 +10694,18 @@
       <c r="U48">
         <v>42763.65</v>
       </c>
+      <c r="V48">
+        <v>55169.5</v>
+      </c>
       <c r="AM48" s="1"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2024</v>
+      </c>
+      <c r="V49">
+        <v>51959</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>